<commit_message>
se arreglo el bug de prelosas macizas
</commit_message>
<xml_diff>
--- a/CONVERTIDOR.xlsx
+++ b/CONVERTIDOR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desktop\Desktop\ddocuments\pythonCAD\autocadAUT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{645C7093-A08B-4732-99C3-DA95478899BF}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C3DF52E-8252-40C3-9BC6-6C9226DBCE01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Convertidor" sheetId="1" r:id="rId1"/>
@@ -1110,7 +1110,7 @@
         <v>7</v>
       </c>
       <c r="G5" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H5" s="57" t="s">
         <v>8</v>
@@ -1195,15 +1195,15 @@
       </c>
       <c r="J8" s="19">
         <f>(G8*VLOOKUP(H8,$C$4:$D$11,2,FALSE))/((G4*VLOOKUP(H4,$C$4:$D$11,2,FALSE)/J4)+IFERROR((G5*VLOOKUP(H5,$C$4:$D$11,2,FALSE)/J5),0)+IFERROR((G6*VLOOKUP(H6,$C$4:$D$11,2,FALSE)/J6),0)+IFERROR((G7*VLOOKUP(H7,$C$4:$D$11,2,FALSE)/J7),0))</f>
-        <v>0.21477500000000002</v>
+        <v>0.60500000000000009</v>
       </c>
       <c r="K8" s="19">
         <f>IF(IF(ABS(J8-_xlfn.CEILING.MATH(J8,0.025))&gt;0,_xlfn.FLOOR.MATH(J8,0.025),_xlfn.CEILING.MATH(J8,0.025))&gt;0.4,0.4,IF(ABS(J8-_xlfn.CEILING.MATH(J8,0.025))&gt;0,_xlfn.FLOOR.MATH(J8,0.025),_xlfn.CEILING.MATH(J8,0.025)))</f>
-        <v>0.2</v>
+        <v>0.4</v>
       </c>
       <c r="L8" s="15">
         <f>VLOOKUP(H8,$C$4:$D$11,2,FALSE)/K8</f>
-        <v>3.55</v>
+        <v>1.7749999999999999</v>
       </c>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
@@ -1227,15 +1227,15 @@
       </c>
       <c r="J9" s="19">
         <f>(G9*VLOOKUP(H9,$C$4:$D$11,2,FALSE))/((G4*VLOOKUP(H4,$C$4:$D$11,2,FALSE)/J4)+IFERROR((G5*VLOOKUP(H5,$C$4:$D$11,2,FALSE)/J5),0)+IFERROR((G6*VLOOKUP(H6,$C$4:$D$11,2,FALSE)/J6),0)+IFERROR((G7*VLOOKUP(H7,$C$4:$D$11,2,FALSE)/J7),0))</f>
-        <v>0.39022500000000004</v>
+        <v>1.0992253521126762</v>
       </c>
       <c r="K9" s="19">
         <f>IF(IF(ABS(J9-_xlfn.CEILING.MATH(J9,0.025))&gt;0,_xlfn.FLOOR.MATH(J9,0.025),_xlfn.CEILING.MATH(J9,0.025))&gt;0.4,0.4,IF(ABS(J9-_xlfn.CEILING.MATH(J9,0.025))&gt;0,_xlfn.FLOOR.MATH(J9,0.025),_xlfn.CEILING.MATH(J9,0.025)))</f>
-        <v>0.375</v>
+        <v>0.4</v>
       </c>
       <c r="L9" s="15">
         <f>VLOOKUP(H9,$C$4:$D$11,2,FALSE)/K9</f>
-        <v>3.44</v>
+        <v>3.2250000000000001</v>
       </c>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
@@ -1259,15 +1259,15 @@
       </c>
       <c r="J10" s="19">
         <f>(G10*VLOOKUP(H10,$C$4:$D$11,2,FALSE))/((G4*VLOOKUP(H4,$C$4:$D$11,2,FALSE)/J4)+IFERROR((G5*VLOOKUP(H5,$C$4:$D$11,2,FALSE)/J5),0)+IFERROR((G6*VLOOKUP(H6,$C$4:$D$11,2,FALSE)/J6),0)+IFERROR((G7*VLOOKUP(H7,$C$4:$D$11,2,FALSE)/J7),0))</f>
-        <v>0.15125000000000002</v>
+        <v>0.42605633802816906</v>
       </c>
       <c r="K10" s="19">
         <f>IF(IF(ABS(J10-_xlfn.CEILING.MATH(J10,0.025))&gt;0,_xlfn.FLOOR.MATH(J10,0.025),_xlfn.CEILING.MATH(J10,0.025))&gt;0.4,0.4,IF(ABS(J10-_xlfn.CEILING.MATH(J10,0.025))&gt;0,_xlfn.FLOOR.MATH(J10,0.025),_xlfn.CEILING.MATH(J10,0.025)))</f>
-        <v>0.15000000000000002</v>
+        <v>0.4</v>
       </c>
       <c r="L10" s="15">
         <f>VLOOKUP(H10,$C$4:$D$11,2,FALSE)/K10</f>
-        <v>3.333333333333333</v>
+        <v>1.25</v>
       </c>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
@@ -1327,7 +1327,7 @@
     </row>
     <row r="15" spans="3:16" x14ac:dyDescent="0.25">
       <c r="G15" s="3">
-        <v>1</v>
+        <v>0</v>
       </c>
       <c r="H15" s="4" t="s">
         <v>8</v>
@@ -1370,15 +1370,15 @@
       </c>
       <c r="J17" s="19">
         <f>(G17*VLOOKUP(H17,$C$4:$D$10,2,FALSE))/((G13*VLOOKUP(H13,$C$4:$D$10,2,FALSE)/J13)+IFERROR((G14*VLOOKUP(H14,$C$4:$D$10,2,FALSE)/J14),0)+IFERROR((G15*VLOOKUP(H15,$C$4:$D$10,2,FALSE)/J15),0)+IFERROR((G16*VLOOKUP(H16,$C$4:$D$10,2,FALSE)/J16),0))</f>
-        <v>0.12330774078218036</v>
+        <v>1.7379082834874011</v>
       </c>
       <c r="K17" s="19">
         <f>IF(IF(ABS(J17-_xlfn.CEILING.MATH(J17,0.025))&gt;0,_xlfn.FLOOR.MATH(J17,0.025),_xlfn.CEILING.MATH(J17,0.025))&gt;0.5,0.5,IF(ABS(J17-_xlfn.CEILING.MATH(J17,0.025))&gt;0,_xlfn.FLOOR.MATH(J17,0.025),_xlfn.CEILING.MATH(J17,0.025)))</f>
-        <v>0.1</v>
+        <v>0.5</v>
       </c>
       <c r="L17" s="15">
         <f>VLOOKUP(H17,$C$4:$D$11,2,FALSE)/K17</f>
-        <v>2.8299999999999996</v>
+        <v>0.56599999999999995</v>
       </c>
     </row>
     <row r="18" spans="3:13" x14ac:dyDescent="0.25">
@@ -1394,15 +1394,15 @@
       </c>
       <c r="J18" s="19">
         <f>(G18*VLOOKUP(H18,$C$4:$D$10,2,FALSE))/((G13*VLOOKUP(H13,$C$4:$D$10,2,FALSE)/J13)+IFERROR((G14*VLOOKUP(H14,$C$4:$D$10,2,FALSE)/J14),0)+IFERROR((G15*VLOOKUP(H15,$C$4:$D$10,2,FALSE)/J15),0)+IFERROR((G16*VLOOKUP(H16,$C$4:$D$10,2,FALSE)/J16),0))</f>
-        <v>0.21785819926180278</v>
+        <v>3.0705093347833943</v>
       </c>
       <c r="K18" s="19">
         <f>IF(IF(ABS(J18-_xlfn.CEILING.MATH(J18,0.025))&gt;0,_xlfn.FLOOR.MATH(J18,0.025),_xlfn.CEILING.MATH(J18,0.025))&gt;0.5,0.5,IF(ABS(J18-_xlfn.CEILING.MATH(J18,0.025))&gt;0,_xlfn.FLOOR.MATH(J18,0.025),_xlfn.CEILING.MATH(J18,0.025)))</f>
-        <v>0.2</v>
+        <v>0.5</v>
       </c>
       <c r="L18" s="15">
         <f>VLOOKUP(H18,$C$4:$D$11,2,FALSE)/K18</f>
-        <v>2.5</v>
+        <v>1</v>
       </c>
     </row>
     <row r="19" spans="3:13" x14ac:dyDescent="0.25">
@@ -1418,15 +1418,15 @@
       </c>
       <c r="J19" s="19">
         <f>(G19*VLOOKUP(H19,$C$4:$D$10,2,FALSE))/((G13*VLOOKUP(H13,$C$4:$D$10,2,FALSE)/J13)+IFERROR((G14*VLOOKUP(H14,$C$4:$D$10,2,FALSE)/J14),0)+IFERROR((G15*VLOOKUP(H15,$C$4:$D$10,2,FALSE)/J15),0)+IFERROR((G16*VLOOKUP(H16,$C$4:$D$10,2,FALSE)/J16),0))</f>
-        <v>0.30935864295175991</v>
+        <v>4.3601232553924198</v>
       </c>
       <c r="K19" s="19">
         <f>IF(IF(ABS(J19-_xlfn.CEILING.MATH(J19,0.025))&gt;0,_xlfn.FLOOR.MATH(J19,0.025),_xlfn.CEILING.MATH(J19,0.025))&gt;0.5,0.5,IF(ABS(J19-_xlfn.CEILING.MATH(J19,0.025))&gt;0,_xlfn.FLOOR.MATH(J19,0.025),_xlfn.CEILING.MATH(J19,0.025)))</f>
-        <v>0.30000000000000004</v>
+        <v>0.5</v>
       </c>
       <c r="L19" s="15">
         <f>VLOOKUP(H19,$C$4:$D$11,2,FALSE)/K19</f>
-        <v>2.3666666666666663</v>
+        <v>1.42</v>
       </c>
     </row>
     <row r="20" spans="3:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
prelosa aligerada de 20 completado
</commit_message>
<xml_diff>
--- a/CONVERTIDOR.xlsx
+++ b/CONVERTIDOR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desktop\Desktop\ddocuments\pythonCAD\autocadAUT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6C3DF52E-8252-40C3-9BC6-6C9226DBCE01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FD45F71B-67D6-4F36-94EA-0E4B59929432}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Convertidor" sheetId="1" r:id="rId1"/>
@@ -1110,7 +1110,7 @@
         <v>7</v>
       </c>
       <c r="G5" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H5" s="57" t="s">
         <v>8</v>
@@ -1195,15 +1195,15 @@
       </c>
       <c r="J8" s="19">
         <f>(G8*VLOOKUP(H8,$C$4:$D$11,2,FALSE))/((G4*VLOOKUP(H4,$C$4:$D$11,2,FALSE)/J4)+IFERROR((G5*VLOOKUP(H5,$C$4:$D$11,2,FALSE)/J5),0)+IFERROR((G6*VLOOKUP(H6,$C$4:$D$11,2,FALSE)/J6),0)+IFERROR((G7*VLOOKUP(H7,$C$4:$D$11,2,FALSE)/J7),0))</f>
-        <v>0.60500000000000009</v>
+        <v>0.21477500000000002</v>
       </c>
       <c r="K8" s="19">
         <f>IF(IF(ABS(J8-_xlfn.CEILING.MATH(J8,0.025))&gt;0,_xlfn.FLOOR.MATH(J8,0.025),_xlfn.CEILING.MATH(J8,0.025))&gt;0.4,0.4,IF(ABS(J8-_xlfn.CEILING.MATH(J8,0.025))&gt;0,_xlfn.FLOOR.MATH(J8,0.025),_xlfn.CEILING.MATH(J8,0.025)))</f>
-        <v>0.4</v>
+        <v>0.2</v>
       </c>
       <c r="L8" s="15">
         <f>VLOOKUP(H8,$C$4:$D$11,2,FALSE)/K8</f>
-        <v>1.7749999999999999</v>
+        <v>3.55</v>
       </c>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
@@ -1227,15 +1227,15 @@
       </c>
       <c r="J9" s="19">
         <f>(G9*VLOOKUP(H9,$C$4:$D$11,2,FALSE))/((G4*VLOOKUP(H4,$C$4:$D$11,2,FALSE)/J4)+IFERROR((G5*VLOOKUP(H5,$C$4:$D$11,2,FALSE)/J5),0)+IFERROR((G6*VLOOKUP(H6,$C$4:$D$11,2,FALSE)/J6),0)+IFERROR((G7*VLOOKUP(H7,$C$4:$D$11,2,FALSE)/J7),0))</f>
-        <v>1.0992253521126762</v>
+        <v>0.39022500000000004</v>
       </c>
       <c r="K9" s="19">
         <f>IF(IF(ABS(J9-_xlfn.CEILING.MATH(J9,0.025))&gt;0,_xlfn.FLOOR.MATH(J9,0.025),_xlfn.CEILING.MATH(J9,0.025))&gt;0.4,0.4,IF(ABS(J9-_xlfn.CEILING.MATH(J9,0.025))&gt;0,_xlfn.FLOOR.MATH(J9,0.025),_xlfn.CEILING.MATH(J9,0.025)))</f>
-        <v>0.4</v>
+        <v>0.375</v>
       </c>
       <c r="L9" s="15">
         <f>VLOOKUP(H9,$C$4:$D$11,2,FALSE)/K9</f>
-        <v>3.2250000000000001</v>
+        <v>3.44</v>
       </c>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
@@ -1259,15 +1259,15 @@
       </c>
       <c r="J10" s="19">
         <f>(G10*VLOOKUP(H10,$C$4:$D$11,2,FALSE))/((G4*VLOOKUP(H4,$C$4:$D$11,2,FALSE)/J4)+IFERROR((G5*VLOOKUP(H5,$C$4:$D$11,2,FALSE)/J5),0)+IFERROR((G6*VLOOKUP(H6,$C$4:$D$11,2,FALSE)/J6),0)+IFERROR((G7*VLOOKUP(H7,$C$4:$D$11,2,FALSE)/J7),0))</f>
-        <v>0.42605633802816906</v>
+        <v>0.15125000000000002</v>
       </c>
       <c r="K10" s="19">
         <f>IF(IF(ABS(J10-_xlfn.CEILING.MATH(J10,0.025))&gt;0,_xlfn.FLOOR.MATH(J10,0.025),_xlfn.CEILING.MATH(J10,0.025))&gt;0.4,0.4,IF(ABS(J10-_xlfn.CEILING.MATH(J10,0.025))&gt;0,_xlfn.FLOOR.MATH(J10,0.025),_xlfn.CEILING.MATH(J10,0.025)))</f>
-        <v>0.4</v>
+        <v>0.15000000000000002</v>
       </c>
       <c r="L10" s="15">
         <f>VLOOKUP(H10,$C$4:$D$11,2,FALSE)/K10</f>
-        <v>1.25</v>
+        <v>3.333333333333333</v>
       </c>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
@@ -1327,7 +1327,7 @@
     </row>
     <row r="15" spans="3:16" x14ac:dyDescent="0.25">
       <c r="G15" s="3">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="H15" s="4" t="s">
         <v>8</v>
@@ -1370,15 +1370,15 @@
       </c>
       <c r="J17" s="19">
         <f>(G17*VLOOKUP(H17,$C$4:$D$10,2,FALSE))/((G13*VLOOKUP(H13,$C$4:$D$10,2,FALSE)/J13)+IFERROR((G14*VLOOKUP(H14,$C$4:$D$10,2,FALSE)/J14),0)+IFERROR((G15*VLOOKUP(H15,$C$4:$D$10,2,FALSE)/J15),0)+IFERROR((G16*VLOOKUP(H16,$C$4:$D$10,2,FALSE)/J16),0))</f>
-        <v>1.7379082834874011</v>
+        <v>0.12330774078218036</v>
       </c>
       <c r="K17" s="19">
         <f>IF(IF(ABS(J17-_xlfn.CEILING.MATH(J17,0.025))&gt;0,_xlfn.FLOOR.MATH(J17,0.025),_xlfn.CEILING.MATH(J17,0.025))&gt;0.5,0.5,IF(ABS(J17-_xlfn.CEILING.MATH(J17,0.025))&gt;0,_xlfn.FLOOR.MATH(J17,0.025),_xlfn.CEILING.MATH(J17,0.025)))</f>
-        <v>0.5</v>
+        <v>0.1</v>
       </c>
       <c r="L17" s="15">
         <f>VLOOKUP(H17,$C$4:$D$11,2,FALSE)/K17</f>
-        <v>0.56599999999999995</v>
+        <v>2.8299999999999996</v>
       </c>
     </row>
     <row r="18" spans="3:13" x14ac:dyDescent="0.25">
@@ -1394,15 +1394,15 @@
       </c>
       <c r="J18" s="19">
         <f>(G18*VLOOKUP(H18,$C$4:$D$10,2,FALSE))/((G13*VLOOKUP(H13,$C$4:$D$10,2,FALSE)/J13)+IFERROR((G14*VLOOKUP(H14,$C$4:$D$10,2,FALSE)/J14),0)+IFERROR((G15*VLOOKUP(H15,$C$4:$D$10,2,FALSE)/J15),0)+IFERROR((G16*VLOOKUP(H16,$C$4:$D$10,2,FALSE)/J16),0))</f>
-        <v>3.0705093347833943</v>
+        <v>0.21785819926180278</v>
       </c>
       <c r="K18" s="19">
         <f>IF(IF(ABS(J18-_xlfn.CEILING.MATH(J18,0.025))&gt;0,_xlfn.FLOOR.MATH(J18,0.025),_xlfn.CEILING.MATH(J18,0.025))&gt;0.5,0.5,IF(ABS(J18-_xlfn.CEILING.MATH(J18,0.025))&gt;0,_xlfn.FLOOR.MATH(J18,0.025),_xlfn.CEILING.MATH(J18,0.025)))</f>
-        <v>0.5</v>
+        <v>0.2</v>
       </c>
       <c r="L18" s="15">
         <f>VLOOKUP(H18,$C$4:$D$11,2,FALSE)/K18</f>
-        <v>1</v>
+        <v>2.5</v>
       </c>
     </row>
     <row r="19" spans="3:13" x14ac:dyDescent="0.25">
@@ -1418,15 +1418,15 @@
       </c>
       <c r="J19" s="19">
         <f>(G19*VLOOKUP(H19,$C$4:$D$10,2,FALSE))/((G13*VLOOKUP(H13,$C$4:$D$10,2,FALSE)/J13)+IFERROR((G14*VLOOKUP(H14,$C$4:$D$10,2,FALSE)/J14),0)+IFERROR((G15*VLOOKUP(H15,$C$4:$D$10,2,FALSE)/J15),0)+IFERROR((G16*VLOOKUP(H16,$C$4:$D$10,2,FALSE)/J16),0))</f>
-        <v>4.3601232553924198</v>
+        <v>0.30935864295175991</v>
       </c>
       <c r="K19" s="19">
         <f>IF(IF(ABS(J19-_xlfn.CEILING.MATH(J19,0.025))&gt;0,_xlfn.FLOOR.MATH(J19,0.025),_xlfn.CEILING.MATH(J19,0.025))&gt;0.5,0.5,IF(ABS(J19-_xlfn.CEILING.MATH(J19,0.025))&gt;0,_xlfn.FLOOR.MATH(J19,0.025),_xlfn.CEILING.MATH(J19,0.025)))</f>
-        <v>0.5</v>
+        <v>0.30000000000000004</v>
       </c>
       <c r="L19" s="15">
         <f>VLOOKUP(H19,$C$4:$D$11,2,FALSE)/K19</f>
-        <v>1.42</v>
+        <v>2.3666666666666663</v>
       </c>
     </row>
     <row r="20" spans="3:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
bloques de texto arreglado
</commit_message>
<xml_diff>
--- a/CONVERTIDOR.xlsx
+++ b/CONVERTIDOR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desktop\Desktop\ddocuments\pythonCAD\autocadAUT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{02D00777-5B4C-4282-9030-208E13FE6968}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{00518748-957C-4C87-8BF3-BE5ACFEF4EF0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1950" yWindow="1950" windowWidth="21600" windowHeight="11295" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Convertidor" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="149" uniqueCount="47">
   <si>
     <t>Acero</t>
   </si>
@@ -1087,14 +1087,14 @@
       <c r="G4" s="20">
         <v>1</v>
       </c>
-      <c r="H4" s="21" t="s">
-        <v>4</v>
+      <c r="H4" s="21">
+        <v>8</v>
       </c>
       <c r="I4" s="22" t="s">
         <v>5</v>
       </c>
       <c r="J4" s="23">
-        <v>0.15</v>
+        <v>0.60499999999999998</v>
       </c>
       <c r="O4" s="1"/>
       <c r="P4" s="1"/>
@@ -1117,7 +1117,7 @@
         <v>5</v>
       </c>
       <c r="J5" s="6">
-        <v>0.6</v>
+        <v>0.3</v>
       </c>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
@@ -1134,13 +1134,13 @@
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="4" t="s">
-        <v>8</v>
+        <v>6</v>
       </c>
       <c r="I6" s="5" t="s">
         <v>5</v>
       </c>
       <c r="J6" s="6">
-        <v>0.4</v>
+        <v>0.6</v>
       </c>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>
@@ -1191,17 +1191,17 @@
       <c r="I8" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="J8" s="19">
+      <c r="J8" s="19" t="e">
         <f>(G8*VLOOKUP(H8,$C$4:$D$11,2,FALSE))/((G4*VLOOKUP(H4,$C$4:$D$11,2,FALSE)/J4)+IFERROR((G5*VLOOKUP(H5,$C$4:$D$11,2,FALSE)/J5),0)+IFERROR((G6*VLOOKUP(H6,$C$4:$D$11,2,FALSE)/J6),0)+IFERROR((G7*VLOOKUP(H7,$C$4:$D$11,2,FALSE)/J7),0))</f>
-        <v>0.15</v>
-      </c>
-      <c r="K8" s="19">
+        <v>#N/A</v>
+      </c>
+      <c r="K8" s="19" t="e">
         <f>IF(IF(ABS(J8-_xlfn.CEILING.MATH(J8,0.025))&gt;0,_xlfn.FLOOR.MATH(J8,0.025),_xlfn.CEILING.MATH(J8,0.025))&gt;0.4,0.4,IF(ABS(J8-_xlfn.CEILING.MATH(J8,0.025))&gt;0,_xlfn.FLOOR.MATH(J8,0.025),_xlfn.CEILING.MATH(J8,0.025)))</f>
-        <v>0.15000000000000002</v>
-      </c>
-      <c r="L8" s="15">
+        <v>#N/A</v>
+      </c>
+      <c r="L8" s="15" t="e">
         <f>VLOOKUP(H8,$C$4:$D$11,2,FALSE)/K8</f>
-        <v>4.7333333333333325</v>
+        <v>#N/A</v>
       </c>
       <c r="N8" s="1"/>
       <c r="O8" s="1"/>
@@ -1223,17 +1223,17 @@
       <c r="I9" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="J9" s="19">
+      <c r="J9" s="19" t="e">
         <f>(G9*VLOOKUP(H9,$C$4:$D$11,2,FALSE))/((G4*VLOOKUP(H4,$C$4:$D$11,2,FALSE)/J4)+IFERROR((G5*VLOOKUP(H5,$C$4:$D$11,2,FALSE)/J5),0)+IFERROR((G6*VLOOKUP(H6,$C$4:$D$11,2,FALSE)/J6),0)+IFERROR((G7*VLOOKUP(H7,$C$4:$D$11,2,FALSE)/J7),0))</f>
-        <v>0.27253521126760566</v>
-      </c>
-      <c r="K9" s="19">
+        <v>#N/A</v>
+      </c>
+      <c r="K9" s="19" t="e">
         <f>IF(IF(ABS(J9-_xlfn.CEILING.MATH(J9,0.025))&gt;0,_xlfn.FLOOR.MATH(J9,0.025),_xlfn.CEILING.MATH(J9,0.025))&gt;0.4,0.4,IF(ABS(J9-_xlfn.CEILING.MATH(J9,0.025))&gt;0,_xlfn.FLOOR.MATH(J9,0.025),_xlfn.CEILING.MATH(J9,0.025)))</f>
-        <v>0.25</v>
-      </c>
-      <c r="L9" s="15">
+        <v>#N/A</v>
+      </c>
+      <c r="L9" s="15" t="e">
         <f>VLOOKUP(H9,$C$4:$D$11,2,FALSE)/K9</f>
-        <v>5.16</v>
+        <v>#N/A</v>
       </c>
       <c r="N9" s="1"/>
       <c r="O9" s="1"/>
@@ -1255,17 +1255,17 @@
       <c r="I10" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="J10" s="19">
+      <c r="J10" s="19" t="e">
         <f>(G10*VLOOKUP(H10,$C$4:$D$11,2,FALSE))/((G4*VLOOKUP(H4,$C$4:$D$11,2,FALSE)/J4)+IFERROR((G5*VLOOKUP(H5,$C$4:$D$11,2,FALSE)/J5),0)+IFERROR((G6*VLOOKUP(H6,$C$4:$D$11,2,FALSE)/J6),0)+IFERROR((G7*VLOOKUP(H7,$C$4:$D$11,2,FALSE)/J7),0))</f>
-        <v>0.10563380281690141</v>
-      </c>
-      <c r="K10" s="19">
+        <v>#N/A</v>
+      </c>
+      <c r="K10" s="19" t="e">
         <f>IF(IF(ABS(J10-_xlfn.CEILING.MATH(J10,0.025))&gt;0,_xlfn.FLOOR.MATH(J10,0.025),_xlfn.CEILING.MATH(J10,0.025))&gt;0.4,0.4,IF(ABS(J10-_xlfn.CEILING.MATH(J10,0.025))&gt;0,_xlfn.FLOOR.MATH(J10,0.025),_xlfn.CEILING.MATH(J10,0.025)))</f>
-        <v>0.1</v>
-      </c>
-      <c r="L10" s="15">
+        <v>#N/A</v>
+      </c>
+      <c r="L10" s="15" t="e">
         <f>VLOOKUP(H10,$C$4:$D$11,2,FALSE)/K10</f>
-        <v>5</v>
+        <v>#N/A</v>
       </c>
       <c r="N10" s="1"/>
       <c r="O10" s="1"/>
@@ -1313,14 +1313,14 @@
       <c r="G14" s="3">
         <v>1</v>
       </c>
-      <c r="H14" s="4" t="s">
-        <v>4</v>
+      <c r="H14" s="4">
+        <v>8</v>
       </c>
       <c r="I14" s="5" t="s">
         <v>5</v>
       </c>
       <c r="J14" s="6">
-        <v>0.15</v>
+        <v>0.60499999999999998</v>
       </c>
     </row>
     <row r="15" spans="3:16" x14ac:dyDescent="0.25">
@@ -1366,15 +1366,15 @@
       </c>
       <c r="J17" s="19">
         <f>(G17*VLOOKUP(H17,$C$4:$D$10,2,FALSE))/((G13*VLOOKUP(H13,$C$4:$D$10,2,FALSE)/J13)+IFERROR((G14*VLOOKUP(H14,$C$4:$D$10,2,FALSE)/J14),0)+IFERROR((G15*VLOOKUP(H15,$C$4:$D$10,2,FALSE)/J15),0)+IFERROR((G16*VLOOKUP(H16,$C$4:$D$10,2,FALSE)/J16),0))</f>
-        <v>7.6021746082507183E-2</v>
+        <v>-0.28000000000000003</v>
       </c>
       <c r="K17" s="19">
         <f>IF(IF(ABS(J17-_xlfn.CEILING.MATH(J17,0.025))&gt;0,_xlfn.FLOOR.MATH(J17,0.025),_xlfn.CEILING.MATH(J17,0.025))&gt;0.5,0.5,IF(ABS(J17-_xlfn.CEILING.MATH(J17,0.025))&gt;0,_xlfn.FLOOR.MATH(J17,0.025),_xlfn.CEILING.MATH(J17,0.025)))</f>
-        <v>7.5000000000000011E-2</v>
+        <v>-0.30000000000000004</v>
       </c>
       <c r="L17" s="15">
         <f>VLOOKUP(H17,$C$4:$D$11,2,FALSE)/K17</f>
-        <v>3.7733333333333325</v>
+        <v>-0.94333333333333313</v>
       </c>
     </row>
     <row r="18" spans="3:13" x14ac:dyDescent="0.25">
@@ -1390,15 +1390,15 @@
       </c>
       <c r="J18" s="19">
         <f>(G18*VLOOKUP(H18,$C$4:$D$10,2,FALSE))/((G13*VLOOKUP(H13,$C$4:$D$10,2,FALSE)/J13)+IFERROR((G14*VLOOKUP(H14,$C$4:$D$10,2,FALSE)/J14),0)+IFERROR((G15*VLOOKUP(H15,$C$4:$D$10,2,FALSE)/J15),0)+IFERROR((G16*VLOOKUP(H16,$C$4:$D$10,2,FALSE)/J16),0))</f>
-        <v>0.13431403901503036</v>
+        <v>-0.49469964664310967</v>
       </c>
       <c r="K18" s="19">
         <f>IF(IF(ABS(J18-_xlfn.CEILING.MATH(J18,0.025))&gt;0,_xlfn.FLOOR.MATH(J18,0.025),_xlfn.CEILING.MATH(J18,0.025))&gt;0.5,0.5,IF(ABS(J18-_xlfn.CEILING.MATH(J18,0.025))&gt;0,_xlfn.FLOOR.MATH(J18,0.025),_xlfn.CEILING.MATH(J18,0.025)))</f>
-        <v>0.125</v>
+        <v>-0.5</v>
       </c>
       <c r="L18" s="15">
         <f>VLOOKUP(H18,$C$4:$D$11,2,FALSE)/K18</f>
-        <v>4</v>
+        <v>-1</v>
       </c>
     </row>
     <row r="19" spans="3:13" x14ac:dyDescent="0.25">
@@ -1414,15 +1414,15 @@
       </c>
       <c r="J19" s="19">
         <f>(G19*VLOOKUP(H19,$C$4:$D$10,2,FALSE))/((G13*VLOOKUP(H13,$C$4:$D$10,2,FALSE)/J13)+IFERROR((G14*VLOOKUP(H14,$C$4:$D$10,2,FALSE)/J14),0)+IFERROR((G15*VLOOKUP(H15,$C$4:$D$10,2,FALSE)/J15),0)+IFERROR((G16*VLOOKUP(H16,$C$4:$D$10,2,FALSE)/J16),0))</f>
-        <v>0.19072593540134311</v>
+        <v>-0.7024734982332157</v>
       </c>
       <c r="K19" s="19">
         <f>IF(IF(ABS(J19-_xlfn.CEILING.MATH(J19,0.025))&gt;0,_xlfn.FLOOR.MATH(J19,0.025),_xlfn.CEILING.MATH(J19,0.025))&gt;0.5,0.5,IF(ABS(J19-_xlfn.CEILING.MATH(J19,0.025))&gt;0,_xlfn.FLOOR.MATH(J19,0.025),_xlfn.CEILING.MATH(J19,0.025)))</f>
-        <v>0.17500000000000002</v>
+        <v>-0.72500000000000009</v>
       </c>
       <c r="L19" s="15">
         <f>VLOOKUP(H19,$C$4:$D$11,2,FALSE)/K19</f>
-        <v>4.0571428571428569</v>
+        <v>-0.97931034482758605</v>
       </c>
     </row>
     <row r="20" spans="3:13" x14ac:dyDescent="0.25">

</xml_diff>

<commit_message>
neuva interfaz - arreglo de ALIGERADA 2 SENT
</commit_message>
<xml_diff>
--- a/CONVERTIDOR.xlsx
+++ b/CONVERTIDOR.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Desktop\Desktop\ddocuments\pythonCAD\autocadAUT\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1B5C13DA-8658-4873-878A-8CB61DBEF37F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{60A8EB71-AA71-4430-BB16-78D017E5D539}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3120" yWindow="3120" windowWidth="21600" windowHeight="11295" xr2:uid="{F062FB74-701C-424C-8982-2B895B398105}"/>
+    <workbookView xWindow="390" yWindow="390" windowWidth="21600" windowHeight="11295" xr2:uid="{F062FB74-701C-424C-8982-2B895B398105}"/>
   </bookViews>
   <sheets>
     <sheet name="Convertidor" sheetId="4" r:id="rId1"/>
@@ -28,7 +28,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="151" uniqueCount="47">
   <si>
     <t>Acero</t>
   </si>
@@ -1081,14 +1081,14 @@
         <v>7</v>
       </c>
       <c r="G5" s="3"/>
-      <c r="H5" s="4">
-        <v>1</v>
+      <c r="H5" s="4" t="s">
+        <v>3</v>
       </c>
       <c r="I5" s="5" t="s">
         <v>5</v>
       </c>
       <c r="J5" s="6">
-        <v>1.75</v>
+        <v>0.4</v>
       </c>
       <c r="O5" s="1"/>
       <c r="P5" s="1"/>
@@ -1105,13 +1105,13 @@
       </c>
       <c r="G6" s="3"/>
       <c r="H6" s="4" t="s">
-        <v>2</v>
+        <v>3</v>
       </c>
       <c r="I6" s="5" t="s">
         <v>5</v>
       </c>
       <c r="J6" s="6">
-        <v>0.4</v>
+        <v>0.25</v>
       </c>
       <c r="O6" s="1"/>
       <c r="P6" s="1"/>

</xml_diff>